<commit_message>
Working the inventory display dialog
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5D6315-C9EB-428A-96A2-25FA7FB7FEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E851EC-3896-4ABC-8040-D071DADF1EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="438">
   <si>
     <t>r203</t>
   </si>
@@ -199,16 +199,6 @@
   </si>
   <si>
     <t>r219</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r201 Characters&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each character in the game has a combat skill, an endurance value, and a wealth code. Each is rated numerically, with higher numbers being better. If no wealth code is given, it is presumed to be zero.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party includes yourself
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR202' Content='r202' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-;  any followers who join your 'party'; and finally any men, women, creatures, and animals encountered in the course of the game. Characters can be friendly or hostile, intelligent or unintelligent.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When a character joins your party, their vital statistics are noted. You can voluntarily dismiss or abandon members of your party if you wish (sometimes expedient when making an escape or when food/money is short). Any characters encountered simply go on thier way and disappear from the game unless they join your party.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine your own personal characteristics at the start of the game, see
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR202a' Content='r202' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r204 Travel&lt;/Bold&gt;
@@ -3978,6 +3968,26 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='t207' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  and roll one die.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the appropriate line for the terrain type you occupy, read across to the Event References column and use the column listed for that die roll. This will produce a Travel Event Reference specified in the table.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r201 Characters&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Each character in the game has a combat skill, an endurance value, and a wealth code. Each is rated numerically, with higher numbers being better. If no wealth code is given, it is presumed to be zero.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party includes yourself
+ &lt;InlineUIContainer&gt;&lt;Button Content='r202' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+;  any followers who join your 'party'; and finally any men, women, creatures, and animals encountered in the course of the game. Characters can be friendly or hostile, intelligent or unintelligent.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When a character joins your party, their vital statistics are noted. You can voluntarily dismiss or abandon members of your party if you wish (sometimes expedient when making an escape or when food/money is short). Any characters encountered simply go on thier way and disappear from the game unless they join your party.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine your own personal characteristics at the start of the game, see
+ &lt;InlineUIContainer&gt;&lt;Button Content='r202' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r057</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r057 Troll Skin&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;A hugh stone-skinned troll was killed by your party. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you killed the troll, its stone-skin is a valuble item. Whenever you have an opportunity to buy food at a town, castle, temple, or from merchants; you can sell the skin for 50 gold pieces. It is also known that Count Drogat of Drogat Castle will treasure the gift should you manage to get a personal audience with him.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/TrollSkin.gif' Height='300' Width='166'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4358,10 +4368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B218"/>
+  <dimension ref="A1:B219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B175" sqref="B175"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4372,1447 +4382,1447 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>374</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>405</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>346</v>
+        <v>407</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>344</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="34" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>387</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="B38" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B53" s="1" t="s">
+    <row r="63" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58" s="1" t="s">
+    <row r="64" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="B65" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>368</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="B71" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="B72" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="B73" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B79" s="1" t="s">
+    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B80" s="1" t="s">
+    <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B82" s="1" t="s">
+    <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="B88" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="B90" s="1" t="s">
-        <v>153</v>
+        <v>63</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="B92" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="B94" s="1" t="s">
-        <v>154</v>
+        <v>329</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="B96" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="B97" s="1" t="s">
-        <v>156</v>
+        <v>64</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+      <c r="B104" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+    <row r="106" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+      <c r="B106" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+      <c r="B107" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B106" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="B108" s="1" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+      <c r="B112" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B113" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B112" s="1" t="s">
+    <row r="115" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B113" s="1" t="s">
+    <row r="116" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B122" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="124" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>201</v>
+        <v>271</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>99</v>
+        <v>200</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>164</v>
+        <v>434</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>169</v>
@@ -5820,303 +5830,311 @@
     </row>
     <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="B192" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B198" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
+      <c r="B200" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
+      <c r="B201" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B200" s="1" t="s">
+    </row>
+    <row r="202" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="B202" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B203" s="1" t="s">
+      <c r="B205" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A204" s="2" t="s">
+    <row r="206" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A205" s="2" t="s">
+      <c r="B206" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B207" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A206" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B206" s="1" t="s">
+    <row r="208" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A207" s="2" t="s">
+      <c r="B208" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B209" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
+      <c r="B210" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B209" s="1" t="s">
+    </row>
+    <row r="211" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
+      <c r="B211" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B210" s="1" t="s">
+    </row>
+    <row r="212" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
+      <c r="B212" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B211" s="1" t="s">
+    </row>
+    <row r="213" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
+      <c r="B213" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B212" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
+      <c r="B214" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>358</v>
+        <v>219</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>206</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A44:B218">
-    <sortCondition ref="A44:A218"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A45:B219">
+    <sortCondition ref="A45:A219"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixup the inventory dialog
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{291721DF-8140-4D0D-992C-04CBDF97BBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA2DE167-AC35-4D66-BB3A-017C6263704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -3091,44 +3091,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;r192 Resurrection Necklace&lt;/Bold&gt;
-&lt;LineBreak/&gt;
-This necklace of black opals and red rubies holds the secret of a second life. If the wearer dies for any reason, including voluntary suicide, at the end of the day, the character rises from the dead.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The necklace disintegrates as the character revives and thus only works once. The resurrection occurs in the same hex, but the character is now free to select any action on the next day. A character revived by the necklace has a somewhat ghoulish cast and is a bit weaker. Endurance is reduced by one. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the Prince is revived by the necklace having been left for dead, he will have lost all possessions and money. The entire party will have scattered although a lover might return
- &lt;InlineUIContainer&gt;&lt;Button Content='r228' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You learn that such appearances are favored at the Dragot Castle. You can add one if seeking an audience
- &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- with Count Dragot. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Necklace</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;r191 Resistance Ring&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 This ring creates a magic aura around the wearer. Every time the wearer is wounded, roll two die:
@@ -3997,35 +3959,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;r098 Dragon Eye&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You encountered a huge, winged fire-breathing dragon.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you killed the dragon, you cut out its eyes. The dragon eyes are valued by High Priest and increases the chance of securing an audience with them.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-         &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DragonEye</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;r099 Roc Beak&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You encountered the Roc, a giagantic bird which swoops down on your party. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you killed the Roc, you cut off its beak.
@@ -4103,6 +4036,76 @@
     <t>r141</t>
   </si>
   <si>
+    <t>r212m</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;r192 Resurrection Necklace&lt;/Bold&gt;
+&lt;LineBreak/&gt;
+This necklace of black opals and red rubies holds the secret of a second life. If the wearer dies for any reason, including voluntary suicide, at the end of the day, the character rises from the dead.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The necklace disintegrates as the character revives and thus only works once. The resurrection occurs in the same hex, but the character is now free to select any action on the next day. A character revived by the necklace has a somewhat ghoulish cast and is a bit weaker. Endurance is reduced by one. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the Prince is revived by the necklace having been left for dead, he will have lost all possessions and money. The entire party will have scattered although a lover might return
+ &lt;InlineUIContainer&gt;&lt;Button Content='r228' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You learn that such appearances are favored at the Dragot Castle. You can add one if seeking an audience
+ &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ with Count Dragot. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                             &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Necklace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;r098 Dragon Eye&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You encountered a huge, winged fire-breathing dragon.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you killed the dragon, you cut out its eyes. The dragon eyes are valued by High Priest and increases the chance of securing an audience with them.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+    &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DragonEye</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>&lt;Bold&gt;r141 Hydra's Teeth&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -4112,7 +4115,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 You can scatter the teeth at any instant to use them that one time including at the start or during any combat.
 &lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image  Source='../../Images/</t>
+                              &lt;InlineUIContainer&gt;&lt;Image  Source='../../Images/</t>
     </r>
     <r>
       <rPr>
@@ -4134,9 +4137,6 @@
       </rPr>
       <t xml:space="preserve">.gif' Height='200'  Width='200'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
     </r>
-  </si>
-  <si>
-    <t>r212m</t>
   </si>
   <si>
     <r>
@@ -4144,7 +4144,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The gods declare your cause a religious crusade and the Staff of Command is passed into your hands. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+              &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
     </r>
     <r>
       <rPr>
@@ -4174,7 +4174,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The griffon is intelligent and could serve both as a member of your party and as a winged mount for other characters.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You cut off its claws and carried them as an extra possession. They are especially valued by Lady Aeravir of Aeravir Castle, and it may help you gain audience with her.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-         &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
     </r>
     <r>
       <rPr>
@@ -4184,7 +4184,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>GriffonClaws</t>
+      <t>GriffonClaw</t>
     </r>
     <r>
       <rPr>
@@ -4579,7 +4579,7 @@
   <dimension ref="A1:B225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4606,18 +4606,18 @@
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -4630,18 +4630,18 @@
     </row>
     <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4686,18 +4686,18 @@
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4710,39 +4710,39 @@
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>449</v>
@@ -4750,34 +4750,34 @@
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>431</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4790,66 +4790,66 @@
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4921,7 +4921,7 @@
         <v>351</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4929,7 +4929,7 @@
         <v>355</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4937,7 +4937,7 @@
         <v>332</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4945,7 +4945,7 @@
         <v>352</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4953,7 +4953,7 @@
         <v>336</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -4961,7 +4961,7 @@
         <v>337</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>391</v>
+        <v>445</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4993,7 +4993,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5105,7 +5105,7 @@
         <v>24</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5145,7 +5145,7 @@
         <v>29</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5302,7 +5302,7 @@
     </row>
     <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>448</v>
@@ -5313,7 +5313,7 @@
         <v>51</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -6033,7 +6033,7 @@
         <v>200</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mnor fix to Giffon Rules
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince2\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA2DE167-AC35-4D66-BB3A-017C6263704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBC9520B-0B1F-40AD-89C2-81AEF3107BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -4171,9 +4171,8 @@
     <r>
       <t>&lt;Bold&gt;r100 Griffon Claws&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You killed a winged griffon.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The griffon is intelligent and could serve both as a member of your party and as a winged mount for other characters.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You cut off its claws and carried them as an extra possession. They are especially valued by Lady Aeravir of Aeravir Castle, and it may help you gain audience with her.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;LineBreak/&gt;
      &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
     </r>
     <r>
@@ -4579,7 +4578,7 @@
   <dimension ref="A1:B225"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4740,7 +4739,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>440</v>
       </c>

</xml_diff>

<commit_message>
Added the Rules Dialog
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBC9520B-0B1F-40AD-89C2-81AEF3107BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6B1505C9-C6F1-4698-A6F2-B76B612B0A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -357,11 +357,6 @@
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonE147' Content='e147' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r212j  High Priestess Request Audience&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;High Priestess requests an audience
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonE155' Content='e155' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
     <t>r220</t>
   </si>
   <si>
@@ -888,22 +883,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If your wit and wiles exceeds the roll, they let your party pass and the event ends.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, see
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR330' Content='r330' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r328 Pass Tough&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Characters encountered have an unpleasant gleem in their eyes. You try to create a favorable impression anyway..
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If your wit and wiles exceeds the roll, they let your party pass and the event ends.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, see
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR330' Content='r330' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- and subtract one from the die roll there.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r325 Pass with Talk&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You think you can lull their suspicions. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If your wit and wiles equals or exceeds the roll, the encountered characters let your party pass. The event ends.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, see
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR330' Content='r330' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- and add one from the die roll there.</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r315 Begging Escape&lt;/Bold&gt;
@@ -2488,50 +2467,7 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r334' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e339 Convince Hirelings&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Characters encountered look askance at you and will pass you by unless you stop to talk. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you stop to talk, you decide you should convince them to join your party as henchmen. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If you wit and wiles exeeds the die roll, they can join at two gold pieces per day with today's pay due right now. You can hire some instead of all you desire. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you stop to talk but fail to convince them to join as hirelings, roll one die to determine their attitude:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 1,2,3 -
- &lt;InlineUIContainer&gt;&lt;Button Content='r325' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-&lt;LineBreak/&gt; 4,5,6 -
- &lt;InlineUIContainer&gt;&lt;Button Content='r330' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>r203a</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e203a Prison Escape Attempt&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Escape:&lt;/Italic&gt; Prison break! Roll one die for each character in your party who was imprisoned with you. They are part of the escape on 3+. Otherwise, they are unable to join the escape or have already been executed.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If an escape occurs, use the escape rules
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- to determine where you end up. The escape takes the entire day and after you must prepare for the evening meals
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;                                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>JailBreak</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.gif' Height='250'  Width='250'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
-</t>
-    </r>
   </si>
   <si>
     <t>&lt;Bold&gt;r220c Strikes&lt;/Bold&gt;
@@ -2652,16 +2588,6 @@
     <t>r073a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;e073a Hostile Witch&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party must escape
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- immediately. Roll one die for each character in your party including yourself. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If a six occurs, the character is turned into a frog and is lost. If you are turned into a frog; any frog, lover, magician, or friendly witch surviving in your party can turn you back.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, you remain a frog for years and lose the game. 
-&lt;LineBreak/&gt; &lt;LineBreak/&gt;
-                           &lt;InlineUIContainer&gt;&lt;Image Name='Witch' Source='../../Images/Witch.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>r079</t>
   </si>
   <si>
@@ -2788,39 +2714,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e090 Quicksand&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party stumbles into quicksand. Roll one die for each character or mount. If a character is riding a mount, you can roll for both together as a character. Alternatively, you can sacrifice the mount and its load in order to jump from it to safety.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-1,2,3 - Character or mount struggles out of the quicksand and is not harmed.&lt;LineBreak/&gt;
-4 - Character or mount escapes only if another character or mount is already free to pull it out. Otherwise, it sinks and dies.&lt;LineBreak/&gt;
-5 - Character struggles outward using vines and tree routes, but a mount is lost with everything it carries.&lt;LineBreak/&gt;
-6 - Character or mount is trapped in deepest part. They cannot win freedom and are automatically lost with everything carried.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Quicksand</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='150'  Width='150'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;r121 Sunstroke&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The heat of the sun is unexpected. Roll one die for each character and mount in your party. A six means he or it collapses from the sunstroke. Mounts that collapse must be left to die.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Characters that collapse must be carried if possible even if that means other loads must be abandoned per
@@ -3320,36 +3213,6 @@
   </si>
   <si>
     <t>r013a</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;Bold&gt;e013a Rich Peasant Family&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Friendly Approach:&lt;/Italic&gt;The family provides food and lodging as if you are in town with the same penalities if you refuse to pay.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Family may sell horses. Roll one die, and a result of 4 plus means they do. If they have stables, roll again for the number of horses available for sale. Roll one die again and double it for the price per horse. They will sell horses at this rate and will also sell food at 2 food units per gold piece. An unlimited amount of food is available for sale.
-&lt;LineBreak/&gt;
-&lt;LineBreak/&gt;
-                        &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lodging</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif'  Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
   </si>
   <si>
     <t>r097</t>
@@ -4140,35 +4003,6 @@
   </si>
   <si>
     <r>
-      <t>&lt;Bold&gt;e212m Gods Declare Crusade&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The gods declare your cause a religious crusade and the Staff of Command is passed into your hands. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-              &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Staff</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>&lt;Bold&gt;r100 Griffon Claws&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You killed a winged griffon.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You cut off its claws and carried them as an extra possession. They are especially valued by Lady Aeravir of Aeravir Castle, and it may help you gain audience with her.
@@ -4195,6 +4029,172 @@
       </rPr>
       <t>.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;r013a Rich Peasant Family&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Friendly Approach:&lt;/Italic&gt;The family provides food and lodging as if you are in town with the same penalities if you refuse to pay.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Family may sell horses. Roll one die, and a result of 4 plus means they do. If they have stables, roll again for the number of horses available for sale. Roll one die again and double it for the price per horse. They will sell horses at this rate and will also sell food at 2 food units per gold piece. An unlimited amount of food is available for sale.
+&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;
+                        &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lodging</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif'  Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r073a Hostile Witch&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party must escape
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ immediately. Roll one die for each character in your party including yourself. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If a six occurs, the character is turned into a frog and is lost. If you are turned into a frog; any frog, lover, magician, or friendly witch surviving in your party can turn you back.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, you remain a frog for years and lose the game. 
+&lt;LineBreak/&gt; &lt;LineBreak/&gt;
+                           &lt;InlineUIContainer&gt;&lt;Image Name='Witch' Source='../../Images/Witch.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;r090 Quicksand&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party stumbles into quicksand. Roll one die for each character or mount. If a character is riding a mount, you can roll for both together as a character. Alternatively, you can sacrifice the mount and its load in order to jump from it to safety.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1,2,3 - Character or mount struggles out of the quicksand and is not harmed.&lt;LineBreak/&gt;
+4 - Character or mount escapes only if another character or mount is already free to pull it out. Otherwise, it sinks and dies.&lt;LineBreak/&gt;
+5 - Character struggles outward using vines and tree routes, but a mount is lost with everything it carries.&lt;LineBreak/&gt;
+6 - Character or mount is trapped in deepest part. They cannot win freedom and are automatically lost with everything carried.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quicksand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='150'  Width='150'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;r203a Prison Escape Attempt&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Escape:&lt;/Italic&gt; Prison break! Roll one die for each character in your party who was imprisoned with you. They are part of the escape on 3+. Otherwise, they are unable to join the escape or have already been executed.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If an escape occurs, use the escape rules
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ to determine where you end up. The escape takes the entire day and after you must prepare for the evening meals
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;                                   &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JailBreak</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.gif' Height='250'  Width='250'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;Bold&gt;r212m Gods Declare Crusade&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The gods declare your cause a religious crusade and the Staff of Command is passed into your hands. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+              &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Staff</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r326 Pass with Talk&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You think you can lull their suspicions. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If your wit and wiles equals or exceeds the roll, the encountered characters let your party pass. The event ends.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, see
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR330' Content='r330' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ and add one from the die roll there.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r329 Pass Tough&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Characters encountered have an unpleasant gleem in their eyes. You try to create a favorable impression anyway..
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If your wit and wiles exceeds the roll, they let your party pass and the event ends.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, see
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR330' Content='r330' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ and subtract one from the die roll there.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r339 Convince Hirelings&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Characters encountered look askance at you and will pass you by unless you stop to talk. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you stop to talk, you decide you should convince them to join your party as henchmen. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If you wit and wiles exeeds the die roll, they can join at two gold pieces per day with today's pay due right now. You can hire some instead of all you desire. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you stop to talk but fail to convince them to join as hirelings, roll one die to determine their attitude:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 1,2,3 -
+ &lt;InlineUIContainer&gt;&lt;Button Content='r325' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt; 4,5,6 -
+ &lt;InlineUIContainer&gt;&lt;Button Content='r330' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r212j High Priestess Request Audience&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;High Priestess requests an audience
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonE155' Content='e155' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
 </sst>
 </file>
@@ -4577,8 +4577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,394 +4589,394 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>399</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>370</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>381</v>
+        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -4984,7 +4984,7 @@
         <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4992,7 +4992,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5000,7 +5000,7 @@
         <v>18</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -5008,15 +5008,15 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>360</v>
+        <v>444</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5029,50 +5029,50 @@
     </row>
     <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5080,7 +5080,7 @@
         <v>21</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5104,7 +5104,7 @@
         <v>24</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5120,7 +5120,7 @@
         <v>26</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -5128,7 +5128,7 @@
         <v>27</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -5144,7 +5144,7 @@
         <v>29</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5152,7 +5152,7 @@
         <v>30</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -5160,7 +5160,7 @@
         <v>31</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="330" x14ac:dyDescent="0.25">
@@ -5168,7 +5168,7 @@
         <v>32</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5176,7 +5176,7 @@
         <v>33</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -5184,7 +5184,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -5192,7 +5192,7 @@
         <v>35</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -5208,7 +5208,7 @@
         <v>37</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -5272,7 +5272,7 @@
         <v>45</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5280,7 +5280,7 @@
         <v>46</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>71</v>
+        <v>449</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5288,7 +5288,7 @@
         <v>47</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5296,15 +5296,15 @@
         <v>50</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -5312,7 +5312,7 @@
         <v>51</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5320,7 +5320,7 @@
         <v>1</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -5328,7 +5328,7 @@
         <v>5</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5360,7 +5360,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5384,7 +5384,7 @@
         <v>12</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5392,7 +5392,7 @@
         <v>13</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5400,7 +5400,7 @@
         <v>14</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5416,7 +5416,7 @@
         <v>52</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5424,7 +5424,7 @@
         <v>61</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5432,7 +5432,7 @@
         <v>3</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5440,7 +5440,7 @@
         <v>4</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5448,103 +5448,103 @@
         <v>53</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5552,839 +5552,839 @@
         <v>2</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>183</v>
+        <v>446</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>182</v>
+        <v>447</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B220" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>358</v>
+        <v>448</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on e146: FoulBane. Added to EventViewerLodgingMgr to purchase when in hex 2018. Started working how it interacts with Drogat during audience
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{511FB123-57C8-49B8-9001-575408A48203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A1AC0F0-C653-4563-AF90-32D3A65742F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="452">
   <si>
     <t>r203</t>
   </si>
@@ -4195,6 +4195,26 @@
 &lt;Italic&gt; - Raid&lt;/Italic&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 If you select a raid and remain in this hex at the end of today, you may be attacked by a revengful mob tomorrow morning before you have a chance to do your daily action. At that time, roll one die. A result of 5+ results in a peasant mob in hot pursuit.  If any other number occurs, there is no mob or event.</t>
+  </si>
+  <si>
+    <t>r146</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r146 The Secret of Count Dragot&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You learn that Count Drogat, lord of Drogat Castle, is acutally an undead creature who enjoys the suffering, pain, and death of others. This explains why he so often tortures and dismembers felons in his realm.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;He often goes into rages that leave his lands in a reign of terror. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;However, he is very vulnerable to foulbane, a rare plant which can be purchased from the food merchants at Duffyd Temple
+ &lt;InlineUIContainer&gt;&lt;Button Content='2018' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ for one gold piece.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using foulbane, when you attempt to gain an audience
+ &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ with Count Drogat, you add one to your dice roll. If you gain an audience, you can ignore the first audience result dice roll and try again. However, if you wish to roll again, you must abide by the second result regardless of the outcome.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Finally, using the foulbane in Drogat Castle, you can spend a day instead of a normal daily action in arranging for a special theft of the Count's personnel jewels.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, you escape from the hex
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/FoulBane.gif' Name='EncounterEnd' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4575,10 +4595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B225"/>
+  <dimension ref="A1:B226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4851,1545 +4871,1553 @@
         <v>438</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>375</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>340</v>
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>326</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+    <row r="113" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B119" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+    <row r="120" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B120" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
+    <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+    <row r="126" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
+    <row r="127" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
+    <row r="128" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
+    <row r="129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
+    <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
+    <row r="131" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B181" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
+    <row r="182" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B182" s="1" t="s">
         <v>423</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="B194" s="1" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="B198" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
+    <row r="199" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B198" s="1" t="s">
+      <c r="B199" s="1" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B201" s="1" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B203" s="1" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A203" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B206" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A206" s="2" t="s">
+    <row r="207" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="B207" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A207" s="2" t="s">
+    <row r="208" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B208" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
+    <row r="209" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B209" s="1" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="B211" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
+    <row r="212" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="B212" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
+    <row r="213" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B212" s="1" t="s">
+      <c r="B213" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
+    <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="B214" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
+    <row r="215" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="B215" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
+    <row r="216" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B215" s="1" t="s">
+      <c r="B216" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
+    <row r="217" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B217" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A217" s="2" t="s">
+    <row r="218" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B218" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A218" s="2" t="s">
+    <row r="219" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="B219" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A219" s="2" t="s">
+    <row r="220" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B219" s="1" t="s">
+      <c r="B220" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A220" s="2" t="s">
+    <row r="221" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B221" s="1" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A221" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B223" s="1" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B224" s="1" t="s">
+      <c r="B225" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A225" s="2" t="s">
+    <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B226" s="1" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A50:B225">
-    <sortCondition ref="A50:A225"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A51:B226">
+    <sortCondition ref="A51:A226"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Make it easier to identify rotating mounts
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A1AC0F0-C653-4563-AF90-32D3A65742F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD5FD133-96C7-4A42-AF82-D8F334589273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -691,15 +691,6 @@
  as hunting is prohibited in these hexes.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r216a Follower Starvation&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If followers are not fed, they may desert. Roll two dice for each follower, and subtract your wit and wiles from the total. If the result is 4 or more, the chaacter deserts your party. Otherwise, he/she stays and suffers from the character starvation
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you have food units or money to purchase it (in a town, castle, or temple), you cannot voluntarily withhold food from your followers unless you go without yourself as well. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If there is insufficient food for all, either you withhold it from all (including yourself) or share out what is available to all (this prevents the effects of character starvation
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b1' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;).
- However, this does not eliminate the risk of desertion described above with character starvation.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r216b Character Starvation&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If a character goes without food for a day, on the following day, his ability to carry loads
  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR206' Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
@@ -4215,6 +4206,15 @@
  with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                      &lt;InlineUIContainer&gt;&lt;Image Source='../../Images/FoulBane.gif' Name='EncounterEnd' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r216a Follower Starvation&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If followers are not fed, they may desert. Roll two dice for each follower, and subtract your wit and wiles from the total. If the result is 4 or more, the follwer deserts your party. Otherwise, he/she stays and suffers from the character starvation
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you have food units or money to purchase it (in a town, castle, or temple), you cannot voluntarily withhold food from your followers unless you go without yourself as well. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If there is insufficient food for all, either you withhold it from all (including yourself) or share out what is available to all (this prevents the effects of character starvation
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b1' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;).
+ However, this does not eliminate the risk of desertion described above with character starvation.</t>
   </si>
 </sst>
 </file>
@@ -4597,8 +4597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4609,402 +4609,402 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>432</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>450</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -5012,7 +5012,7 @@
         <v>19</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5020,7 +5020,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5028,7 +5028,7 @@
         <v>18</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -5036,15 +5036,15 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5057,50 +5057,50 @@
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5108,7 +5108,7 @@
         <v>21</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5132,7 +5132,7 @@
         <v>24</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5148,7 +5148,7 @@
         <v>26</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -5156,7 +5156,7 @@
         <v>27</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>29</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5180,7 +5180,7 @@
         <v>30</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -5188,7 +5188,7 @@
         <v>31</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="330" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>32</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5204,7 +5204,7 @@
         <v>33</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -5212,7 +5212,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -5236,7 +5236,7 @@
         <v>37</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -5300,7 +5300,7 @@
         <v>45</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5308,7 +5308,7 @@
         <v>46</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5316,7 +5316,7 @@
         <v>47</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5329,10 +5329,10 @@
     </row>
     <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -5340,7 +5340,7 @@
         <v>51</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5348,7 +5348,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -5356,7 +5356,7 @@
         <v>5</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5412,7 +5412,7 @@
         <v>12</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5420,7 +5420,7 @@
         <v>13</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>152</v>
+        <v>451</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5428,7 +5428,7 @@
         <v>14</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5444,7 +5444,7 @@
         <v>52</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5452,7 +5452,7 @@
         <v>61</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5460,7 +5460,7 @@
         <v>3</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5468,7 +5468,7 @@
         <v>4</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5476,7 +5476,7 @@
         <v>53</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5484,7 +5484,7 @@
         <v>71</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5492,7 +5492,7 @@
         <v>72</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5500,7 +5500,7 @@
         <v>73</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5508,7 +5508,7 @@
         <v>74</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5532,7 +5532,7 @@
         <v>77</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5540,7 +5540,7 @@
         <v>78</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5548,7 +5548,7 @@
         <v>80</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -5564,7 +5564,7 @@
         <v>82</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -5580,7 +5580,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5588,7 +5588,7 @@
         <v>86</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5596,7 +5596,7 @@
         <v>87</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5604,7 +5604,7 @@
         <v>88</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>90</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5628,7 +5628,7 @@
         <v>93</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -5644,423 +5644,423 @@
         <v>95</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6068,7 +6068,7 @@
         <v>97</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6076,7 +6076,7 @@
         <v>98</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6084,7 +6084,7 @@
         <v>99</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>100</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6100,7 +6100,7 @@
         <v>101</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6108,7 +6108,7 @@
         <v>102</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6116,7 +6116,7 @@
         <v>103</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6124,7 +6124,7 @@
         <v>104</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6132,7 +6132,7 @@
         <v>105</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6140,7 +6140,7 @@
         <v>106</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6148,7 +6148,7 @@
         <v>107</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6156,7 +6156,7 @@
         <v>108</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6164,7 +6164,7 @@
         <v>109</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6172,7 +6172,7 @@
         <v>110</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6180,7 +6180,7 @@
         <v>111</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6188,7 +6188,7 @@
         <v>112</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6196,7 +6196,7 @@
         <v>113</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6204,7 +6204,7 @@
         <v>114</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6212,7 +6212,7 @@
         <v>115</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -6220,7 +6220,7 @@
         <v>116</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -6228,7 +6228,7 @@
         <v>117</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6236,7 +6236,7 @@
         <v>118</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6244,7 +6244,7 @@
         <v>119</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6252,7 +6252,7 @@
         <v>120</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6260,7 +6260,7 @@
         <v>121</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -6276,7 +6276,7 @@
         <v>124</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6284,7 +6284,7 @@
         <v>125</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6292,7 +6292,7 @@
         <v>126</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -6300,7 +6300,7 @@
         <v>127</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -6332,7 +6332,7 @@
         <v>133</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6364,7 +6364,7 @@
         <v>141</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6380,7 +6380,7 @@
         <v>144</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -6388,7 +6388,7 @@
         <v>145</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -6396,7 +6396,7 @@
         <v>146</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -6404,7 +6404,7 @@
         <v>147</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6412,7 +6412,7 @@
         <v>148</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates from pull down from main
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA2C8D97-977F-4C14-B4FE-4EC9D4D4866E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE7F628-DD8D-4406-A64E-EF7571069F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -2930,12 +2930,6 @@
                &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Overcast.gif' Height='220' Width='480'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r107 Falcon Scout&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the evening meal each day, if you offer the falcon a food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r109 Wild Pegasus&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You encounter a wild Pegasus. Each character in your party is allowed one attempt to capture it.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If the result is 5 plus, the character captures the Pegasus. You may add it as a winged mount to your party.
@@ -3249,6 +3243,12 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
               &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Staff.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r107 Falcon Scout&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the evening meal each day, if you offer the falcon a food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide. You cannot get lost when you have the falcon.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -3617,8 +3617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3795,12 +3795,12 @@
         <v>421</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>385</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>422</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3808,7 +3808,7 @@
         <v>386</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3816,7 +3816,7 @@
         <v>387</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3824,7 +3824,7 @@
         <v>365</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -3832,7 +3832,7 @@
         <v>382</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -3840,7 +3840,7 @@
         <v>373</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3848,7 +3848,7 @@
         <v>372</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3856,7 +3856,7 @@
         <v>376</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -3864,7 +3864,7 @@
         <v>377</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -3872,7 +3872,7 @@
         <v>375</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -3880,7 +3880,7 @@
         <v>394</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -3888,7 +3888,7 @@
         <v>395</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -3896,7 +3896,7 @@
         <v>402</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3904,7 +3904,7 @@
         <v>339</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3912,7 +3912,7 @@
         <v>340</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3928,7 +3928,7 @@
         <v>341</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3936,7 +3936,7 @@
         <v>342</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3944,7 +3944,7 @@
         <v>343</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3952,7 +3952,7 @@
         <v>331</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3960,7 +3960,7 @@
         <v>344</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -3968,7 +3968,7 @@
         <v>345</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3976,7 +3976,7 @@
         <v>348</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3984,7 +3984,7 @@
         <v>328</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -3992,7 +3992,7 @@
         <v>346</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4000,7 +4000,7 @@
         <v>332</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -4008,7 +4008,7 @@
         <v>333</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4016,7 +4016,7 @@
         <v>334</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4024,7 +4024,7 @@
         <v>335</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -4064,7 +4064,7 @@
         <v>351</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4352,7 +4352,7 @@
         <v>396</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="210" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix issue with populated hunting is e050
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\Documents\Visual Studio 2022\Projects\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BE7F628-DD8D-4406-A64E-EF7571069F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CE5E7B3-CC4C-470B-9F1E-A3732CADC550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="15" windowWidth="25440" windowHeight="15390" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -295,16 +295,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If your party rested today in the hex, you can send additional characters to hunt. For each additional character hunting, add one to the skill+endurance level of your hunt. The actual skill and endurance of the additional hunters is not counted. However, if the additional hunters are gides, add one for each guide.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r215c Populated Regions and Hunting&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you must hunt in a farmland hex, each time you roll one die for a possible event, which occurs after the hunt is finished, but before the evening meal is eaten: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 1,2,3,4-Do nothing.
-&lt;LineBreak/&gt; 5-Peasant mob in pursuit
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonE017' Content='e017' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt; 6-Pursued by constabulary
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonE051' Content='e051' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Hunting is prohibited in any hex with a town, castle, or temple.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r216c Mount Starvation&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If animals in a party go without food, their carrying capacity is halved for each day of starvation just like characters. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;When the carrying capacity reaches zero, the mount dies. 
@@ -3249,6 +3239,16 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;At the evening meal each day, if you offer the falcon a food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide. You cannot get lost when you have the falcon.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                         &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r215c Populated Regions and Hunting&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you must hunt in a farmland hex, each time you roll one die for a possible event, which occurs after the hunt is finished, but before the evening meal is eaten: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 1,2,3,4-Do nothing.
+&lt;LineBreak/&gt; 5-Peasant mob in pursuit
+ &lt;InlineUIContainer&gt;&lt;Button Content='e017' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt; 6-Pursued by constabulary
+ &lt;InlineUIContainer&gt;&lt;Button Content='e050' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Hunting is prohibited in any hex with a town, castle, or temple.</t>
   </si>
 </sst>
 </file>
@@ -3617,8 +3617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3629,402 +3629,402 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -4032,7 +4032,7 @@
         <v>19</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4040,7 +4040,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4048,7 +4048,7 @@
         <v>18</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -4056,15 +4056,15 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4077,50 +4077,50 @@
     </row>
     <row r="57" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4128,7 +4128,7 @@
         <v>21</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4152,7 +4152,7 @@
         <v>24</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4168,7 +4168,7 @@
         <v>26</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
         <v>27</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
@@ -4192,7 +4192,7 @@
         <v>29</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4200,7 +4200,7 @@
         <v>30</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4208,7 +4208,7 @@
         <v>31</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="330" x14ac:dyDescent="0.25">
@@ -4216,7 +4216,7 @@
         <v>32</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4224,7 +4224,7 @@
         <v>33</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4232,7 +4232,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4240,7 +4240,7 @@
         <v>35</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4248,7 +4248,7 @@
         <v>36</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4256,7 +4256,7 @@
         <v>37</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4272,7 +4272,7 @@
         <v>39</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4280,7 +4280,7 @@
         <v>40</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4288,7 +4288,7 @@
         <v>41</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4304,7 +4304,7 @@
         <v>43</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4312,7 +4312,7 @@
         <v>44</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4320,7 +4320,7 @@
         <v>45</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4328,7 +4328,7 @@
         <v>46</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4336,7 +4336,7 @@
         <v>47</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4344,15 +4344,15 @@
         <v>50</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4360,7 +4360,7 @@
         <v>51</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4368,7 +4368,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -4376,7 +4376,7 @@
         <v>5</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4400,7 +4400,7 @@
         <v>8</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>63</v>
+        <v>451</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4408,7 +4408,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4432,7 +4432,7 @@
         <v>12</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4440,7 +4440,7 @@
         <v>13</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4448,7 +4448,7 @@
         <v>14</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4456,7 +4456,7 @@
         <v>15</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4464,7 +4464,7 @@
         <v>52</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4472,7 +4472,7 @@
         <v>61</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4480,7 +4480,7 @@
         <v>3</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4488,7 +4488,7 @@
         <v>4</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4496,103 +4496,103 @@
         <v>53</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4600,839 +4600,839 @@
         <v>2</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B219" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B221" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rule for r049
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\happysulla\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FA9E184-461D-4019-8894-8530F3FDA0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C65E13BD-CD0F-4175-919A-D18F30EC037C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -3257,9 +3257,9 @@
     <t>&lt;Bold&gt;r049 Travelling Minstrel&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You have a musician that has joined your party.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If he is fed, he will sing a tale that night that prevents any of your party from deserting no matter what happened today.  This applies even if your followers are not properly fed or lodged.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When at the evening meal, click his image to start him singing to prevent desertions.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When at the evening meal, click his image to start him singing to prevent desertions. However, when he sings, he leaves the next day.
 &lt;LineBreak/&gt; &lt;LineBreak/&gt; 
-                                                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Minstrel.gif' Height='280' Width='140'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                               &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Minstrel.gif' Height='280' Width='140'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -3628,7 +3628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added helper dialog for character stats
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AF51151-AD38-4E97-8399-4C27F38DD632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FF562EA7-8599-41C5-801E-6C8C255A4778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2219,17 +2219,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Escapes across a river are prohibited. However, if your entire party has winged mounts or are able to fly, you can fly over the river and escape that way. Similarly, you cannot escape off the map.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r216 Starvation&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you cannot provide food each day for characters or mounts, startvation will begin to affect their loyalty and performance. Each unit is sufficient to feed one person for one day. Mounts require two units per day if they are unable to forage for their own fodder. In a desert hext with no oasis, the food requirement doubles for men and mounts to represent the need to also carry water supplies.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216a' Content='r216a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Follower Starvation&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Character Starvation&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216c' Content='r216c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Mount Starvation</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r225a Special Possessions&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Sometimes the result of the Treasure Table
  &lt;InlineUIContainer&gt;&lt;Button Content='t226' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
@@ -3272,6 +3261,17 @@
  with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                       &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/CountDrogatJewels.gif' Name='CountDrogatJewels' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r216 Starvation&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you cannot provide food each day for characters or mounts, startvation will begin to affect their loyalty and performance. Each food unit is sufficient to feed one person for one day. Mounts require two units per day if they are unable to forage for their own fodder. In a desert hext with no oasis, the food requirement doubles for men and mounts to represent the need to also carry water supplies.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216a' Content='r216a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Follower Starvation&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Character Starvation&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216c' Content='r216c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Mount Starvation</t>
   </si>
 </sst>
 </file>
@@ -3640,8 +3640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3652,418 +3652,418 @@
   <sheetData>
     <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4071,7 +4071,7 @@
         <v>19</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4079,7 +4079,7 @@
         <v>17</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4100,10 +4100,10 @@
     </row>
     <row r="57" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>24</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4231,7 +4231,7 @@
         <v>29</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4239,7 +4239,7 @@
         <v>30</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4247,7 +4247,7 @@
         <v>31</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="330" x14ac:dyDescent="0.25">
@@ -4255,7 +4255,7 @@
         <v>32</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4263,7 +4263,7 @@
         <v>33</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4271,7 +4271,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4367,7 +4367,7 @@
         <v>46</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4388,10 +4388,10 @@
     </row>
     <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4399,7 +4399,7 @@
         <v>51</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4439,7 +4439,7 @@
         <v>8</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4471,7 +4471,7 @@
         <v>12</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>323</v>
+        <v>455</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4479,7 +4479,7 @@
         <v>13</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4535,7 +4535,7 @@
         <v>53</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4543,7 +4543,7 @@
         <v>70</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4567,7 +4567,7 @@
         <v>73</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4647,7 +4647,7 @@
         <v>85</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4655,7 +4655,7 @@
         <v>86</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5119,7 +5119,7 @@
         <v>195</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5335,7 +5335,7 @@
         <v>123</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5359,7 +5359,7 @@
         <v>126</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -5439,7 +5439,7 @@
         <v>143</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5455,7 +5455,7 @@
         <v>145</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="390" x14ac:dyDescent="0.25">
@@ -5463,7 +5463,7 @@
         <v>146</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added r144i button. Chnaged end condition to win with 500gp anywhere
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FF562EA7-8599-41C5-801E-6C8C255A4778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CED3FFA0-29E3-4DD4-A15F-257FB9D95E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="458">
   <si>
     <t>r203</t>
   </si>
@@ -3272,6 +3272,16 @@
  Character Starvation&lt;LineBreak/&gt;
   &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216c' Content='r216c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  Mount Starvation</t>
+  </si>
+  <si>
+    <t>r144i</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r144i Baron Hauldra Sneak Attack&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You can make a sneak attack on the Baron at night suprising his traditional six bodyguards &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Each has combat skill 6 and endurance 6. Once you kill the bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                           &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/BodyGuard.gif' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -3638,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B228"/>
+  <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,1561 +3932,1569 @@
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>401</v>
+        <v>432</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>435</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>356</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+    <row r="81" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B90" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+    <row r="91" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B93" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>449</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>455</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B106" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+    <row r="110" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B110" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B111" s="1" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B113" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+    <row r="116" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B116" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="118" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B118" s="1" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B122" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B123" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B124" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
+    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B125" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
+    <row r="126" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B126" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
+    <row r="127" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
+    <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B128" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
+    <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B129" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
+    <row r="130" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B130" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
+    <row r="131" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B131" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
+    <row r="132" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B132" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
+    <row r="133" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B133" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+    <row r="134" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B134" s="1" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B184" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
+    <row r="185" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B185" s="1" t="s">
         <v>385</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="B197" s="1" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B201" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
+    <row r="202" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B201" s="1" t="s">
+      <c r="B202" s="1" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B203" s="1" t="s">
+      <c r="B204" s="1" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A204" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B206" s="1" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A206" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B209" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
+    <row r="210" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="B210" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
+    <row r="211" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="B211" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
+    <row r="212" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="B212" s="1" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="B214" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
+    <row r="215" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="B215" s="1" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
+    <row r="216" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B215" s="1" t="s">
+      <c r="B216" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
+    <row r="217" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B217" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A217" s="2" t="s">
+    <row r="218" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B218" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A218" s="2" t="s">
+    <row r="219" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="B219" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A219" s="2" t="s">
+    <row r="220" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B219" s="1" t="s">
+      <c r="B220" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A220" s="2" t="s">
+    <row r="221" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B221" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A221" s="2" t="s">
+    <row r="222" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B221" s="1" t="s">
+      <c r="B222" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A222" s="2" t="s">
+    <row r="223" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B223" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
+    <row r="224" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B224" s="1" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B226" s="1" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A226" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B227" s="1" t="s">
+      <c r="B228" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
+    <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B229" s="1" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:B228">
-    <sortCondition ref="A53:A228"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A54:B229">
+    <sortCondition ref="A54:A229"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix problem with all dead party meembers when plague dust check starts
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE3CB50F-19A8-477C-AF49-97DBA7DA26C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3912FA1-B953-405D-B556-0830F599153B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="82680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -404,12 +404,6 @@
     <t>r227a</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r227a Plague Dust&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die and halve the results rounding upward.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You suffer these many wounds at the end of the day. You will continue to suffer the same number after every day.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine recovery, roll one die after the sickness wounds are inflicted. If this second roll is 4+, you recover. Otherwsie sickness continues.</t>
-  </si>
-  <si>
     <t>r228</t>
   </si>
   <si>
@@ -3282,6 +3276,12 @@
 &lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204e' Content='r204e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossings
 &lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204f' Content='r204f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events and Time
 &lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR206' Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Transport</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r227a Plague Dust&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die and halve the results rounding upward.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You suffer these many wounds at the end of the day. You will continue to suffer the same number after every day.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine recovery, roll one die after the sickness wounds are inflicted. If this second roll is 4+, you recover. Otherwise sickness continues.</t>
   </si>
 </sst>
 </file>
@@ -3650,545 +3650,545 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="231.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="2"/>
+    <col min="2" max="2" width="231.578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="B47" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="360" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B61" s="1" t="s">
+    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="2" t="s">
         <v>23</v>
       </c>
@@ -4204,15 +4204,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="2" t="s">
         <v>25</v>
       </c>
@@ -4220,23 +4220,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="2" t="s">
         <v>28</v>
       </c>
@@ -4244,63 +4244,63 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="2" t="s">
         <v>36</v>
       </c>
@@ -4308,15 +4308,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="2" t="s">
         <v>38</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="2" t="s">
         <v>39</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="2" t="s">
         <v>40</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="2" t="s">
         <v>41</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="2" t="s">
         <v>42</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="2" t="s">
         <v>43</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="2" t="s">
         <v>44</v>
       </c>
@@ -4372,71 +4372,71 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="2" t="s">
         <v>6</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="2" t="s">
         <v>7</v>
       </c>
@@ -4452,23 +4452,23 @@
         <v>61</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="2" t="s">
         <v>10</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="2" t="s">
         <v>11</v>
       </c>
@@ -4484,31 +4484,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="2" t="s">
         <v>15</v>
       </c>
@@ -4516,79 +4516,79 @@
         <v>62</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="2" t="s">
         <v>73</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="2" t="s">
         <v>74</v>
       </c>
@@ -4604,31 +4604,31 @@
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="2" t="s">
         <v>79</v>
       </c>
@@ -4636,15 +4636,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="2" t="s">
         <v>81</v>
       </c>
@@ -4652,844 +4652,844 @@
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
+      <c r="B131" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B132" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B132" s="1" t="s">
+    <row r="134" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B133" s="1" t="s">
+      <c r="B186" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A164" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A168" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A174" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A178" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A183" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A186" s="2" t="s">
+    <row r="187" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="B187" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
+    <row r="188" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="B188" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
+    <row r="189" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B188" s="1" t="s">
+      <c r="B189" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
+    <row r="190" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B189" s="1" t="s">
+      <c r="B190" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A190" s="2" t="s">
+    <row r="191" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="B191" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B192" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B191" s="1" t="s">
+    <row r="193" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A193" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B193" s="1" t="s">
+    <row r="197" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A195" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B195" s="1" t="s">
+    <row r="198" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A206" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A196" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A201" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B201" s="1" t="s">
+    <row r="207" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A202" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A203" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A204" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B204" s="1" t="s">
+    <row r="210" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A205" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A206" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A207" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A208" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B208" s="1" t="s">
+    <row r="211" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A220" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A222" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A223" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B223" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A215" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B215" s="1" t="s">
+    <row r="224" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A224" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A225" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A217" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A218" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A219" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A220" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A221" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A222" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A223" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A224" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A225" s="2" t="s">
+    <row r="226" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A226" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B225" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A226" s="2" t="s">
+      <c r="B226" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A227" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B226" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
+      <c r="B227" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A228" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B227" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
+      <c r="B228" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A229" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B228" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A229" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="B229" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tutorial to allow Fun Options or Original Options
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\BarbarianPrince\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3912FA1-B953-405D-B556-0830F599153B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CECA023-67A1-4205-A2D4-A133DBD5C8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="82680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -3202,7 +3202,72 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Hunting is prohibited in any hex with a town, castle, or temple.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r200 How to Play&lt;/Bold&gt;
+    <t>r049</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r049 Travelling Minstrel&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You have a musician that has joined your party.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If he is fed, he will sing a tale that night that prevents any of your party from deserting no matter what happened today.  This applies even if your followers are not properly fed or lodged.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When at the evening meal, click his image to start him singing to prevent desertions. However, when he sings, he leaves the next day.
+&lt;LineBreak/&gt; &lt;LineBreak/&gt; 
+                               &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Minstrel.gif' Height='280' Width='140'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r146a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e146a Stealing Count Drogat Jewels&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the foulbane in Drogat Castle, you can spend a &lt;Bold&gt;Steal Gems&lt;/Bold&gt; action instead of a normal daily action in arranging for a special theft of the Count's personnel jewels.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, you escape from the hex
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                      &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/CountDrogatJewels.gif' Name='CountDrogatJewels' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r216 Starvation&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you cannot provide food each day for characters or mounts, startvation will begin to affect their loyalty and performance. Each food unit is sufficient to feed one person for one day. Mounts require two units per day if they are unable to forage for their own fodder. In a desert hext with no oasis, the food requirement doubles for men and mounts to represent the need to also carry water supplies.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216a' Content='r216a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Follower Starvation&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Character Starvation&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216c' Content='r216c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Mount Starvation</t>
+  </si>
+  <si>
+    <t>r144i</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r144i Baron Hauldra Sneak Attack&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You can make a sneak attack on the Baron at night suprising his traditional six bodyguards &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Each has combat skill 6 and endurance 6. Once you kill the bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                           &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/BodyGuard.gif' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r204 Travel&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You can travel to new hexes as a daily action
+ &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+. You travel by moving your party across the map, hex by hex. You cannot skip or jump any hex unless a special event allows it.
+&lt;LineBreak/&gt;
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204a' Content='r204a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Speeds
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205' Content='r205' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Getting Lost
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204b' Content='r204b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204c' Content='r204c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Roads
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204d' Content='r204d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Airborne Travel
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204e' Content='r204e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossings
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204f' Content='r204f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events and Time
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR206' Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Transport</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r227a Plague Dust&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die and halve the results rounding upward.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You suffer these many wounds at the end of the day. You will continue to suffer the same number after every day.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine recovery, roll one die after the sickness wounds are inflicted. If this second roll is 4+, you recover. Otherwise sickness continues.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r200 How to Play&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Barbarian Prince&lt;/Italic&gt; is a dungeon cawler, self-paced, solo game. You play the game in days. Each day starts with your selecting a daily action
  &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 , such as traveling to a new hex on the map. Depending on the action selected, you will be referred to a chart, where you roll one or two die. The dice roll and the chart may then indicate a special event section, when you then resolve.
@@ -3216,72 +3281,7 @@
 . You may also have additional characters
  &lt;InlineUIContainer&gt;&lt;Button Content='r201' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  join your party. These additinal characters are especially useful in fights, although some may have special knowleddge or abiliities useful in certain events. Magicians, wizards, witches, priests, and monks are especially useful people to have in your party. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;All events are self explanatory, and refer to the main rules dialogs that describes how they are resolved.</t>
-  </si>
-  <si>
-    <t>r049</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r049 Travelling Minstrel&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You have a musician that has joined your party.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If he is fed, he will sing a tale that night that prevents any of your party from deserting no matter what happened today.  This applies even if your followers are not properly fed or lodged.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When at the evening meal, click his image to start him singing to prevent desertions. However, when he sings, he leaves the next day.
-&lt;LineBreak/&gt; &lt;LineBreak/&gt; 
-                               &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Minstrel.gif' Height='280' Width='140'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>r146a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e146a Stealing Count Drogat Jewels&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the foulbane in Drogat Castle, you can spend a &lt;Bold&gt;Steal Gems&lt;/Bold&gt; action instead of a normal daily action in arranging for a special theft of the Count's personnel jewels.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, you escape from the hex
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                      &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/CountDrogatJewels.gif' Name='CountDrogatJewels' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r216 Starvation&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you cannot provide food each day for characters or mounts, startvation will begin to affect their loyalty and performance. Each food unit is sufficient to feed one person for one day. Mounts require two units per day if they are unable to forage for their own fodder. In a desert hext with no oasis, the food requirement doubles for men and mounts to represent the need to also carry water supplies.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216a' Content='r216a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Follower Starvation&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Character Starvation&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216c' Content='r216c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Mount Starvation</t>
-  </si>
-  <si>
-    <t>r144i</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r144i Baron Hauldra Sneak Attack&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You can make a sneak attack on the Baron at night suprising his traditional six bodyguards &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Each has combat skill 6 and endurance 6. Once you kill the bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                           &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/BodyGuard.gif' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r204 Travel&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You can travel to new hexes as a daily action
- &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-. You travel by moving your party across the map, hex by hex. You cannot skip or jump any hex unless a special event allows it.
-&lt;LineBreak/&gt;
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204a' Content='r204a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Speeds
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205' Content='r205' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Getting Lost
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204b' Content='r204b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204c' Content='r204c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Roads
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204d' Content='r204d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Airborne Travel
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204e' Content='r204e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossings
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204f' Content='r204f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events and Time
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR206' Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Transport</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r227a Plague Dust&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die and halve the results rounding upward.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You suffer these many wounds at the end of the day. You will continue to suffer the same number after every day.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine recovery, roll one die after the sickness wounds are inflicted. If this second roll is 4+, you recover. Otherwise sickness continues.</t>
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;All events are self explanatory. Click the rules button that brings up dialogs on details. </t>
   </si>
 </sst>
 </file>
@@ -3650,17 +3650,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.15625" style="2"/>
-    <col min="2" max="2" width="231.578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="231.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>342</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>348</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>364</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>369</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>325</v>
       </c>
@@ -3700,15 +3700,15 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>373</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>385</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>355</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>356</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>359</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>358</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>361</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>374</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>375</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>362</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>363</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>365</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>387</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>386</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>388</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>379</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>380</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>381</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>382</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>360</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>377</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>368</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>367</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>371</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>372</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="360" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" ht="375" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>370</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>389</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>390</v>
       </c>
@@ -3932,15 +3932,15 @@
         <v>427</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="36" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>397</v>
       </c>
@@ -3948,15 +3948,15 @@
         <v>428</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>334</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>335</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>332</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>336</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>337</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>338</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>326</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>339</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>340</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>343</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>323</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>341</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>327</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>328</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>329</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>330</v>
       </c>
@@ -4084,15 +4084,15 @@
         <v>443</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>17</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>18</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="360" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>0</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>346</v>
       </c>
@@ -4124,15 +4124,15 @@
         <v>444</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>201</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>202</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>203</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>205</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>206</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>207</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>21</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
@@ -4196,7 +4196,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>23</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>24</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>25</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>26</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>27</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>28</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>29</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>31</v>
       </c>
@@ -4268,7 +4268,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="316.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>32</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>33</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>35</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>36</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>37</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>38</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>39</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>40</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>41</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>42</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>43</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>44</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>391</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>51</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>1</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="288" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>6</v>
       </c>
@@ -4444,7 +4444,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>7</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>8</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>9</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>10</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>11</v>
       </c>
@@ -4484,15 +4484,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>13</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>14</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>15</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>52</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>60</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>3</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>4</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>53</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>69</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>70</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>71</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>72</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>73</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>74</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>75</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>76</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>78</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>79</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>80</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>81</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>84</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>85</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>86</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>88</v>
       </c>
@@ -4692,15 +4692,15 @@
         <v>184</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>90</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>91</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>92</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>213</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>215</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>216</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>217</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>218</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>219</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>220</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>221</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>222</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>223</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>224</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>225</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>226</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>227</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>228</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>229</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>230</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>231</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>232</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>233</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>234</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>235</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>236</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>237</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>238</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>239</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>240</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>241</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>242</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>243</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>244</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>245</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>246</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>247</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>248</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>249</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>250</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>251</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>252</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>253</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>254</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>255</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>256</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>257</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>258</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>259</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>260</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>261</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>262</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>263</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>264</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>193</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>94</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>95</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>96</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>97</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>98</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>99</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>100</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>101</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>102</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>103</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>104</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>105</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>106</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>107</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>108</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>109</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>110</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>111</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>112</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>113</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>114</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>115</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>116</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>117</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>118</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>119</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>121</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>122</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>123</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>124</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>125</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>126</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>129</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>130</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>132</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>134</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>136</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>138</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>139</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>141</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>142</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>143</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>144</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
Got ClickOnce deployment to work
</commit_message>
<xml_diff>
--- a/Documentation/Rules.xlsx
+++ b/Documentation/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\BarbarianPrince\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CECA023-67A1-4205-A2D4-A133DBD5C8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{99A9786C-5DAB-4C9D-A4A9-F6CBAE792ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -2709,12 +2709,72 @@
  However, this does not eliminate the risk of desertion described above with character starvation.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r182 Gift of Charm&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;This is a small item of no real value, but it does have a magic aura. You can give this gift to any characters you encounter as part of any talk or negiotiaton.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When you use it, you can then roll a second and a third time of that option. You select the die result you want.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Once given away, the gift is gone and useless unless the receiver later fights you in combat and you kill the defenders. Then, you can recover the gift as part of the defender's possessions. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/CharmGift.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    <t>&lt;Bold&gt;r215c Populated Regions and Hunting&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you must hunt in a farmland hex, each time you roll one die for a possible event, which occurs after the hunt is finished, but before the evening meal is eaten: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 1,2,3,4-Do nothing.
+&lt;LineBreak/&gt; 5-Peasant mob in pursuit
+ &lt;InlineUIContainer&gt;&lt;Button Content='e017' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt; 6-Pursued by constabulary
+ &lt;InlineUIContainer&gt;&lt;Button Content='e050' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Hunting is prohibited in any hex with a town, castle, or temple.</t>
+  </si>
+  <si>
+    <t>r049</t>
+  </si>
+  <si>
+    <t>r146a</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r216 Starvation&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you cannot provide food each day for characters or mounts, startvation will begin to affect their loyalty and performance. Each food unit is sufficient to feed one person for one day. Mounts require two units per day if they are unable to forage for their own fodder. In a desert hext with no oasis, the food requirement doubles for men and mounts to represent the need to also carry water supplies.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216a' Content='r216a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Follower Starvation&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Character Starvation&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216c' Content='r216c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ Mount Starvation</t>
+  </si>
+  <si>
+    <t>r144i</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r204 Travel&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You can travel to new hexes as a daily action
+ &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+. You travel by moving your party across the map, hex by hex. You cannot skip or jump any hex unless a special event allows it.
+&lt;LineBreak/&gt;
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204a' Content='r204a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Speeds
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205' Content='r205' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Getting Lost
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204b' Content='r204b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204c' Content='r204c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Roads
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204d' Content='r204d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Airborne Travel
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204e' Content='r204e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossings
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204f' Content='r204f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events and Time
+&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR206' Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Transport</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r227a Plague Dust&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die and halve the results rounding upward.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You suffer these many wounds at the end of the day. You will continue to suffer the same number after every day.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine recovery, roll one die after the sickness wounds are inflicted. If this second roll is 4+, you recover. Otherwise sickness continues.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r200 How to Play&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Barbarian Prince&lt;/Italic&gt; is a dungeon cawler, self-paced, solo game. You play the game in days. Each day starts with your selecting a daily action
+ &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, such as traveling to a new hex on the map. Depending on the action selected, you will be referred to a chart, where you roll one or two die. The dice roll and the chart may then indicate a special event section, when you then resolve.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;After all events are resolved for your daily action, you must eat your main evening meal as described in the food rules
+ &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+, and if in a town, castle, or temple hex; you must also purchase lodging
+ &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR217' Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;This ends the day, and you continue play with the start of the next day, where you select another action. The game continues until either you are killed or 70 days (10 weeks) elapse. If you have not won before the 70 days ends, the game is automatically lost!
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Many events may lead to fighting, described in the combat rules
+ &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+. You may also have additional characters
+ &lt;InlineUIContainer&gt;&lt;Button Content='r201' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ join your party. These additinal characters are especially useful in fights, although some may have special knowleddge or abiliities useful in certain events. Magicians, wizards, witches, priests, and monks are especially useful people to have in your party. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;All events are self explanatory. Click the rules button that brings up dialogs on details. </t>
   </si>
   <si>
     <t>&lt;Bold&gt;r013a Rich Peasant Family&lt;/Bold&gt;
@@ -2722,7 +2782,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Family may sell horses. Roll one die, and a result of 4 plus means they do. If they have stables, roll again for the number of horses available for sale. Roll one die again and double it for the price per horse. They will sell horses at this rate and will also sell food at 2 food units per gold piece. An unlimited amount of food is available for sale.
 &lt;LineBreak/&gt;
 &lt;LineBreak/&gt;
-                        &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Lodging.gif'  Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                        &lt;InlineUIContainer&gt;&lt;Image Source='../images/Lodging.gif'  Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r018 Priest&lt;/Bold&gt;
@@ -2737,7 +2797,15 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  with the high priest of any temple marked on the map, but may with high priest of any secret unmarked temples that you find.
 &lt;LineBreak/&gt;
-                              &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Priest.gif'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                              &lt;InlineUIContainer&gt;&lt;Image Source='../images/Priest.gif'  Height='150' Width='150'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r049 Travelling Minstrel&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;You have a musician that has joined your party.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If he is fed, he will sing a tale that night that prevents any of your party from deserting no matter what happened today.  This applies even if your followers are not properly fed or lodged.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When at the evening meal, click his image to start him singing to prevent desertions. However, when he sings, he leaves the next day.
+&lt;LineBreak/&gt; &lt;LineBreak/&gt; 
+                               &lt;InlineUIContainer&gt;&lt;Image Source='../images/Minstrel.gif' Height='280' Width='140'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r051 Bandits&lt;/Bold&gt;
@@ -2746,14 +2814,14 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The number of bandits exceeds the number of characters in your party by two.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;One of the bandits is the leader with combat skill 6, endurance 6, and wealth 15. The rest have combat skill 5, endurance 4, and wealth 1.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Bandit.gif' Height='300' Width='180'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                 &lt;InlineUIContainer&gt;&lt;Image Source='../images/Bandit.gif' Height='300' Width='180'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r057 Troll Skin&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;A hugh stone-skinned troll was killed by your party. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you killed the troll, its stone-skin is a valuble item. Whenever you have an opportunity to buy food at a town, castle, temple, or from merchants; you can sell the skin for 50 gold pieces. It is also known that Count Drogat of Drogat Castle will treasure the gift should you manage to get a personal audience with him.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/TrollSkin.gif' Height='300' Width='166'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                &lt;InlineUIContainer&gt;&lt;Image Source='../images/TrollSkin.gif' Height='300' Width='166'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r073a Hostile Witch&lt;/Bold&gt;
@@ -2763,7 +2831,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If a six occurs, the character is turned into a frog and is lost. If you are turned into a frog; any frog, lover, magician, or friendly witch surviving in your party can turn you back.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Otherwise, you remain a frog for years and lose the game. 
 &lt;LineBreak/&gt; &lt;LineBreak/&gt;
-                           &lt;InlineUIContainer&gt;&lt;Image Name='Witch' Source='../bin/Images/Witch.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                           &lt;InlineUIContainer&gt;&lt;Image Name='Witch' Source='../images/Witch.gif' Height='300' Width='240'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r085 Narrow Ledges&lt;/Bold&gt;
@@ -2772,7 +2840,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you personally slip or your mount falls over the edge, you are presumed to catch a ledge somewhere down the cliff and survive. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die and add one for the number of wounds suffered in the fall. Also, roll one die to see if your party finds you. A 5 or higher indicates they do. Any lower roll means the rest of your party does not find you and disappears with all the mounts, possessions, and wealth they are carrying.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                              &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/NarrowLedge.gif' Height='125'  Width='250'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                              &lt;InlineUIContainer&gt;&lt;Image Source='../images/NarrowLedge.gif' Height='125'  Width='250'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r088 Rockfall&lt;/Bold&gt;
@@ -2782,7 +2850,7 @@
  &lt;LineBreak/&gt;5 - Character suffers one wound from flying rock chips. Mounts without a rider are caught by a rolling bolder, breaks a leg, and must be killed.
  &lt;LineBreak/&gt;6 - Character hit by heavy rock. Roll one die and add one for wounds suffered. Mounts without rider are hit and killed instantly. All of its load are buried beneath the rocks and are lost.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-          &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/LandSlide.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+          &lt;InlineUIContainer&gt;&lt;Image Source='../images/LandSlide.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r090 Quicksand&lt;/Bold&gt;
@@ -2793,7 +2861,7 @@
 5 - Character struggles outward using vines and tree routes, but a mount is lost with everything it carries.&lt;LineBreak/&gt;
 6 - Character or mount is trapped in deepest part. They cannot win freedom and are automatically lost with everything carried.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Quicksand.gif' Height='150'  Width='150'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/Quicksand.gif' Height='150'  Width='150'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r091 Poison Snake&lt;/Bold&gt;
@@ -2802,13 +2870,13 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r343' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  suffers snakebit poison wounds. Roll one die for the number of poison wounds received.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-              &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Snake.gif' Height='280'  Width='400'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+              &lt;InlineUIContainer&gt;&lt;Image Source='../images/Snake.gif' Height='280'  Width='400'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e094a Crocodiles in River&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Your party is attacked by very large and very hungry crocodiles. They achieve surprise in combat  &lt;InlineUIContainer&gt;&lt;Button Content='r310' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. They have combat skill 4 and endurance of 6. Roll one die for the number fo crocs.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                 &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Crocs.gif' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                 &lt;InlineUIContainer&gt;&lt;Image Source='../images/Crocs.gif' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r095 Mounts at Risk&lt;/Bold&gt;
@@ -2818,7 +2886,7 @@
 &lt;LineBreak/&gt; 5: Mount failing. Unless you rest &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; , it  dies tomorrow.
 &lt;LineBreak/&gt; 6: Mount in serious condition. It dies immediately.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                 &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/MountTired.gif' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                 &lt;InlineUIContainer&gt;&lt;Image Source='../images/MountTired.gif' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r096 Mounts Sick&lt;/Bold&gt;
@@ -2829,20 +2897,20 @@
  3: Mount still failing. Roll again at end of tomorrow.&lt;LineBreak/&gt;
  4,5,6: Mount dies now
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                 &lt;InlineUIContainer&gt;&lt;Image Name='MountsDie' Source='../bin/Images/MountsDie.gif' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                 &lt;InlineUIContainer&gt;&lt;Image Name='MountsDie' Source='../images/MountsDie.gif' Height='200' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r097 Marsh Gas and Rot&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Your entire party has unwittingly travelled into an area full of flesh-rot disease and mind-destroying marsh gas. Roll one die for each character. If a one results, the character escapes. Any other result means the character dies a mindless and raving idiot while his flesh rots from his bones before his eyes.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-         &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/FleshRot.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+         &lt;InlineUIContainer&gt;&lt;Image Source='../images/FleshRot.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r098 Dragon Eye&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You encountered a huge, winged fire-breathing dragon.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Since you killed the dragon, you cut out its eyes. The dragon eyes are valued by High Priest and increases the chance of securing an audience with them.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-    &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/DragonEye.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+    &lt;InlineUIContainer&gt;&lt;Image Source='../images/DragonEye.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r099 Roc Beak&lt;/Bold&gt;
@@ -2853,14 +2921,14 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 In addition, the beak can be sold to any merchant, or in any town/castle/temple whenever you buy food. The beak is worth 35gp.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-         &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/RocBeak.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+         &lt;InlineUIContainer&gt;&lt;Image Source='../images/RocBeak.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r100 Griffon Claws&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You killed a winged griffon.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You cut off its claws and carried them as an extra possession. They are especially valued by Lady Aeravir of Aeravir Castle, and it may help you gain audience with her.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/GriffonClaw.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+     &lt;InlineUIContainer&gt;&lt;Image Source='../images/GriffonClaw.gif' Height='250' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r106 Heavy Overcast&lt;/Bold&gt;
@@ -2868,14 +2936,20 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die for each character or unridden mount. A six means that the character or mount disppears into the overcast and is lost from your party.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Finally, the overcast will force you and the remainder of your party to land in the new hex. No futher travel is possible today. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-               &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Overcast.gif' Height='220' Width='480'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+               &lt;InlineUIContainer&gt;&lt;Image Source='../images/Overcast.gif' Height='220' Width='480'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r107 Falcon Scout&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the evening meal each day, if you offer the falcon a food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide. You cannot get lost when you have the falcon.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Source='../images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r109 Wild Pegasus&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You encounter a wild Pegasus. Each character in your party is allowed one attempt to capture it.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die. If the result is 5 plus, the character captures the Pegasus. You may add it as a winged mount to your party.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Pegasus.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                 &lt;InlineUIContainer&gt;&lt;Image Source='../images/Pegasus.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r111 Storm Demon Attacks&lt;/Bold&gt;
@@ -2883,7 +2957,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You are unable to block the attack, and your entire party is blown away to be lost or killed. Your winged mount is killed, but your carried wealth and possessions are intact. The rest of your party is lost.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You crash in an adjacent hex. Roll one die for the number of wounds suffered.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                              &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/StormDemon.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                              &lt;InlineUIContainer&gt;&lt;Image Source='../images/StormDemon.gif' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r121 Sunstroke&lt;/Bold&gt;
@@ -2893,19 +2967,19 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you suffer sunstroke and are not carried, your party leaves you behind and disappear. You suffer wounds equal to one die roll. You revive in time for the evening meal
  &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Click image to continue.
 &lt;LineBreak/&gt;
-                                    &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Sun5.gif' Height='250'  Width='250' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                    &lt;InlineUIContainer&gt;&lt;Image Source='../images/Sun5.gif' Height='250'  Width='250' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r123a Knight at the Bridge Refusal&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You refused the combat and end travel for the day. Roll one die for each character in your party. A six means they desert you for cowardice.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                         &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/BlackKnightRefuse.gif' Height='200'  Width='350' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                         &lt;InlineUIContainer&gt;&lt;Image Source='../images/BlackKnightRefuse.gif' Height='200'  Width='350' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r125 Raft Overturns&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The raft is caught in an eddy, hits a rock, and overturns. Everyone in your party including mounts swims to shore. However, all wealth and all possessions are lost.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/RaftWhiteWater5.gif' Height='225'  Width='400' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/RaftWhiteWater5.gif' Height='225'  Width='400' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r126 Raft Caught in Current&lt;/Bold&gt;
@@ -2913,14 +2987,14 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die for each mount and the characters in your party. A six indicates it is lost overboard and drowns. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you fall overboard, you can swim to shore, losing all your wealth, possessions, and mount. You party disppears downriver on the raft and is lost to you.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/RaftWhiteWater3.gif' Height='225'  Width='400' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/RaftWhiteWater3.gif' Height='225'  Width='400' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r127 Raft in Rough Water&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Your raft hits white water. All food stores piled on it are lost overboard.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;All characters, mounts, wealth, and possession are saved. Raft continues its journey safely.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                             &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/RaftWhiteWater1.gif' Height='300'  Width='300' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                             &lt;InlineUIContainer&gt;&lt;Image Source='../images/RaftWhiteWater1.gif' Height='300'  Width='300' &gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r128 Merchant&lt;/Bold&gt;
@@ -2944,7 +3018,7 @@
   12 - Learn unique secrets from the merchant. See
  &lt;InlineUIContainer&gt;&lt;Button Content='e162' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;
-                                          &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Merchant.gif' Height='150'  Width='93'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                          &lt;InlineUIContainer&gt;&lt;Image Source='../images/Merchant.gif' Height='150'  Width='93'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Bold&gt;r129 Merchant Caravan&lt;/Bold&gt;
@@ -2971,7 +3045,7 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='e147' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.&lt;LineBreak/&gt;
   12 - Caravan passed a nearby ruins yesterday. Roll one die for which hex: 1-N,2-NE,3-SE, 4-S,5-SW,6-NW.&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;
-                           &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Caravan.gif' Height='150'  Width='300'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;	</t>
+                           &lt;InlineUIContainer&gt;&lt;Image Source='../images/Caravan.gif' Height='150'  Width='300'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;	</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Bold&gt;r140 Magic Box Found&lt;/Bold&gt;
@@ -2985,7 +3059,7 @@
  5 - Random Possession&lt;LineBreak/&gt;
  6 - Nothing but rubbish
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image  Source='../bin/Images/BoxUnopened.gif' Name='BoxUnopened' Height='200'  Width='200'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+                                 &lt;InlineUIContainer&gt;&lt;Image  Source='../images/BoxUnopened.gif' Name='BoxUnopened' Height='200'  Width='200'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Bold&gt;r141 Hydra's Teeth&lt;/Bold&gt;
@@ -2996,7 +3070,14 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 You can scatter the teeth at any instant to use them that one time including at the start or during any combat.
 &lt;LineBreak/&gt;
-                              &lt;InlineUIContainer&gt;&lt;Image  Source='../bin/Images/Teeth.gif' Height='200'  Width='200'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+                              &lt;InlineUIContainer&gt;&lt;Image  Source='../images/Teeth.gif' Height='200'  Width='200'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r144i Baron Hauldra Sneak Attack&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You can make a sneak attack on the Baron at night suprising his traditional six bodyguards &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Each has combat skill 6 and endurance 6. Once you kill the bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                           &lt;InlineUIContainer&gt;&lt;Image Source='../images/BodyGuard.gif' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r146 The Secret of Count Dragot&lt;/Bold&gt;
@@ -3013,14 +3094,23 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/FoulBane.gif' Name='EncounterEnd' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                     &lt;InlineUIContainer&gt;&lt;Image Source='../images/FoulBane.gif' Name='EncounterEnd' Height='250' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;e146a Stealing Count Drogat Jewels&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the foulbane in Drogat Castle, you can spend a &lt;Bold&gt;Steal Gems&lt;/Bold&gt; action instead of a normal daily action in arranging for a special theft of the Count's personnel jewels.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, you escape from the hex
+ &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                      &lt;InlineUIContainer&gt;&lt;Image Source='../images/CountDrogatJewels.gif' Name='CountDrogatJewels' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r180 Healing Potion&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;This potion can be applied once to any character including yourself at the end of the day after the evening meal
  &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 . The potion immediately cures all wounds except poison wounds.&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-          &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/PotionHeal.gif' Name='Possession' Height='500' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+          &lt;InlineUIContainer&gt;&lt;Image Source='../images/PotionHeal.gif' Name='Possession' Height='500' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r181 Cure Poison Vial&lt;/Bold&gt;
@@ -3028,7 +3118,15 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 . It will cure all poisoned wounds overnight. Only poison wounds are cured. It has no effect on regular wounds. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-          &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/PotionCure.gif' Name='Possession' Height='500' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+          &lt;InlineUIContainer&gt;&lt;Image Source='../images/PotionCure.gif' Name='Possession' Height='500' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r182 Gift of Charm&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;This is a small item of no real value, but it does have a magic aura. You can give this gift to any characters you encounter as part of any talk or negiotiaton.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When you use it, you can then roll a second and a third time of that option. You select the die result you want.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Once given away, the gift is gone and useless unless the receiver later fights you in combat and you kill the defenders. Then, you can recover the gift as part of the defender's possessions. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/CharmGift.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r183 Endurance Sash&lt;/Bold&gt;
@@ -3036,14 +3134,14 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The effect is permanet as long as you retain your possessions. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;You cannot wear more than one sash. Additional ones may be given to other characters in your party. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-        &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Sash.gif' Name='Possession' Height='30' Width='550'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+        &lt;InlineUIContainer&gt;&lt;Image Source='../images/Sash.gif' Name='Possession' Height='30' Width='550'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r184 Resistance Talisman&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The gold talisman allows you to resist all magic spells and attacks. Whenever magic is used, you can call upon the talisman to negate it.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;However, the talisman may be unable to contain a strong spell. Each time it is used, roll one die. A result of 6 means the spell is stopped and the talisman is shuttered and broken in the process.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/TalismanResistance.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/TalismanResistance.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r185 Poison Drug&lt;/Bold&gt;
@@ -3053,21 +3151,21 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;After a combat where the poisoned weapon is used, roll one die. A result of 6 means the poison has worn off and the weapon returns to normal.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Since a character often has multiple weapons, he has the option of using his poisoned weapon or a normal weapon as desired. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/PoisonDrug.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/PoisonDrug.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r186 Magic Sword&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;A character can carry this special sword amoung his weapons. The magic sword adds one to the combat skill of the character with it.
 In addition, the blade's magic means that every wound it inflicts counts as a poisoned wound. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Sword.gif' Name='Possession' Height='170' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/Sword.gif' Name='Possession' Height='170' Width='500'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r187 Anti-poison Amulet&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;This protects against all poisoned wounds. Any poison wound inflicted is ignored if the target has the amulet. Normal wounds still take effect. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Each time a poison wound is prevented, roll two die. If the result is 12, the amulet has reached its limit. It cannot absorb more poison and must be discarded. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-         &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/AmuletAntiPoison.gif' Name='Possession' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+         &lt;InlineUIContainer&gt;&lt;Image Source='../images/AmuletAntiPoison.gif' Name='Possession' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r188 Pegasus Mount&lt;/Bold&gt;
@@ -3083,7 +3181,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 You can use the Pegasus as a normal mount on the ground if desired. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Pegasus.gif' Name='Possession' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/Pegasus.gif' Name='Possession' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r188a Pegasus Talisman&lt;/Bold&gt;
@@ -3093,7 +3191,7 @@
 Whenever you have any magician, wizard, witch, priest, or monk in your party; they can help you use the talisman to call upon an actual Pegasus winged mount. It will immediately appear and serve as your mount
  &lt;InlineUIContainer&gt;&lt;Button Content='r188' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/TalismanPegasus.gif' Name='Possession' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/TalismanPegasus.gif' Name='Possession' Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;e189 Charisma Talisman&lt;/Bold&gt;
@@ -3101,7 +3199,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;This talisman does not improve your wit and wiles when trying to evade, hide, attack, or surprise. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;Like many magical devices, this talisman's spell may eventually wear out. After each use, roll two die. If the total is 12, it has worn out and must be discared. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                        &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/TalismanCharisma.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                        &lt;InlineUIContainer&gt;&lt;Image Source='../images/TalismanCharisma.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r190 Nerve Gas Bomb&lt;/Bold&gt;
@@ -3117,7 +3215,7 @@
 The jar with the gas is rather heavy. It counts as one load to transport
  &lt;InlineUIContainer&gt;&lt;Button Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/NerveGasBomb.gif' Name='Possession' Height='300' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/NerveGasBomb.gif' Name='Possession' Height='300' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r191 Resistance Ring&lt;/Bold&gt;
@@ -3130,7 +3228,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The ring can be used to ward poison wounds like normal wounds. The ring can also be used to ward magic attacks against the wearer, but it will not protect others in the party. In a magic attack, two rolls must be made, and the single worst result to the wearer is applied.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                  &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/RingResistence.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                  &lt;InlineUIContainer&gt;&lt;Image Source='../images/RingResistence.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r192 Resurrection Necklace&lt;/Bold&gt;
@@ -3146,7 +3244,7 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r211' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  with Count Dragot. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                             &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Necklace.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                             &lt;InlineUIContainer&gt;&lt;Image Source='../images/Necklace.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r193 Shield of Light&lt;/Bold&gt;
@@ -3154,7 +3252,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of each combat where the shield is used, roll one die. If a 6 is rolled, the shield is so banged and damaged by battle that it is now useless.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;To preserve the shield, you may elect to not use it in some combats. You can change your mind during the battle but must then check for damage after the battle. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                 &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Shield.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                 &lt;InlineUIContainer&gt;&lt;Image Source='../images/Shield.gif' Name='Possession' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r194 Royal Helm of Northlands&lt;/Bold&gt;
@@ -3166,7 +3264,7 @@
  towns with the helm, you will instantly be hailed as the rightful King of the Northlands and win the game!
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;In the meantime, possession of the helm increases your stature and self-confidence. Increase your wit and wiles by one.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Helmet.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/Helmet.gif' Name='Possession' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;Bold&gt;r203a Prison Escape Attempt&lt;/Bold&gt;
@@ -3175,7 +3273,7 @@
  &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
  to determine where you end up. The escape takes the entire day and after you must prepare for the evening meals
  &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;                                   &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/JailBreak.gif' Height='250'  Width='250'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;                                   &lt;InlineUIContainer&gt;&lt;Image Source='../images/JailBreak.gif' Height='250'  Width='250'&gt; &lt;/Image&gt;&lt;/InlineUIContainer&gt;
 </t>
   </si>
   <si>
@@ -3183,105 +3281,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The gods declare your cause a religious crusade and the Staff of Command is passed into your hands. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;If you bring this possession to any hex north of the, you will command instant obedience throughout the Norhlands, regain your throne, and win the game! 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-              &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Staff.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r107 Falcon Scout&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the evening meal each day, if you offer the falcon a food unit, roll the die. If you roll anyhing other than a six, the falcon will remain throughout tomorrow with your party as a guide. You cannot get lost when you have the falcon.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Falcon.gif' Height='188' Width='250'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r215c Populated Regions and Hunting&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you must hunt in a farmland hex, each time you roll one die for a possible event, which occurs after the hunt is finished, but before the evening meal is eaten: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 1,2,3,4-Do nothing.
-&lt;LineBreak/&gt; 5-Peasant mob in pursuit
- &lt;InlineUIContainer&gt;&lt;Button Content='e017' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt; 6-Pursued by constabulary
- &lt;InlineUIContainer&gt;&lt;Button Content='e050' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Hunting is prohibited in any hex with a town, castle, or temple.</t>
-  </si>
-  <si>
-    <t>r049</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r049 Travelling Minstrel&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You have a musician that has joined your party.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If he is fed, he will sing a tale that night that prevents any of your party from deserting no matter what happened today.  This applies even if your followers are not properly fed or lodged.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When at the evening meal, click his image to start him singing to prevent desertions. However, when he sings, he leaves the next day.
-&lt;LineBreak/&gt; &lt;LineBreak/&gt; 
-                               &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/Minstrel.gif' Height='280' Width='140'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>r146a</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;e146a Stealing Count Drogat Jewels&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Using the foulbane in Drogat Castle, you can spend a &lt;Bold&gt;Steal Gems&lt;/Bold&gt; action instead of a normal daily action in arranging for a special theft of the Count's personnel jewels.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;At the end of the day, you escape from the hex
- &lt;InlineUIContainer&gt;&lt;Button Content='r218' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- with wealth 110. However, you can never return to the castle hex due to the Count's anger. In the process of the theft, you might acquire magic items as part of the wealth 110 check. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                      &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/CountDrogatJewels.gif' Name='CountDrogatJewels' Height='300' Width='300'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r216 Starvation&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;If you cannot provide food each day for characters or mounts, startvation will begin to affect their loyalty and performance. Each food unit is sufficient to feed one person for one day. Mounts require two units per day if they are unable to forage for their own fodder. In a desert hext with no oasis, the food requirement doubles for men and mounts to represent the need to also carry water supplies.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216a' Content='r216a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Follower Starvation&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216b' Content='r216b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Character Starvation&lt;LineBreak/&gt;
-  &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR216c' Content='r216c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- Mount Starvation</t>
-  </si>
-  <si>
-    <t>r144i</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r144i Baron Hauldra Sneak Attack&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You can make a sneak attack on the Baron at night suprising his traditional six bodyguards &lt;InlineUIContainer&gt; &lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Each has combat skill 6 and endurance 6. Once you kill the bodyguards, you can attack the Baron who has combat skill 6 and endurance 8. The Baron strikes first in combat. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                           &lt;InlineUIContainer&gt;&lt;Image Source='../bin/Images/BodyGuard.gif' Height='350' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r204 Travel&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You can travel to new hexes as a daily action
- &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-. You travel by moving your party across the map, hex by hex. You cannot skip or jump any hex unless a special event allows it.
-&lt;LineBreak/&gt;
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204a' Content='r204a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Speeds
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR205' Content='r205' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Getting Lost
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204b' Content='r204b' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204c' Content='r204c' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Roads
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204d' Content='r204d' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Airborne Travel
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204e' Content='r204e' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; River Crossings
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR204f' Content='r204f' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Travel Events and Time
-&lt;LineBreak/&gt; &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR206' Content='r206' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Transport</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r227a Plague Dust&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Roll one die and halve the results rounding upward.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;You suffer these many wounds at the end of the day. You will continue to suffer the same number after every day.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;To determine recovery, roll one die after the sickness wounds are inflicted. If this second roll is 4+, you recover. Otherwise sickness continues.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r200 How to Play&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;&lt;Italic&gt;Barbarian Prince&lt;/Italic&gt; is a dungeon cawler, self-paced, solo game. You play the game in days. Each day starts with your selecting a daily action
- &lt;InlineUIContainer&gt;&lt;Button Content='r203' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, such as traveling to a new hex on the map. Depending on the action selected, you will be referred to a chart, where you roll one or two die. The dice roll and the chart may then indicate a special event section, when you then resolve.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;After all events are resolved for your daily action, you must eat your main evening meal as described in the food rules
- &lt;InlineUIContainer&gt;&lt;Button Content='r215' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-, and if in a town, castle, or temple hex; you must also purchase lodging
- &lt;InlineUIContainer&gt;&lt;Button Name='myButtonR217' Content='r217' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;This ends the day, and you continue play with the start of the next day, where you select another action. The game continues until either you are killed or 70 days (10 weeks) elapse. If you have not won before the 70 days ends, the game is automatically lost!
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Many events may lead to fighting, described in the combat rules
- &lt;InlineUIContainer&gt;&lt;Button Content='r220' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-. You may also have additional characters
- &lt;InlineUIContainer&gt;&lt;Button Content='r201' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
- join your party. These additinal characters are especially useful in fights, although some may have special knowleddge or abiliities useful in certain events. Magicians, wizards, witches, priests, and monks are especially useful people to have in your party. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;All events are self explanatory. Click the rules button that brings up dialogs on details. </t>
+              &lt;InlineUIContainer&gt;&lt;Image Source='../images/Staff.gif' Height='300' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -3650,8 +3650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3681,7 +3681,7 @@
         <v>364</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -3689,7 +3689,7 @@
         <v>369</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -3702,10 +3702,10 @@
     </row>
     <row r="6" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>448</v>
+        <v>400</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -3713,7 +3713,7 @@
         <v>373</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3721,7 +3721,7 @@
         <v>385</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>403</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3729,7 +3729,7 @@
         <v>355</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
         <v>359</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3753,7 +3753,7 @@
         <v>358</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -3761,7 +3761,7 @@
         <v>361</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -3769,7 +3769,7 @@
         <v>374</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3777,7 +3777,7 @@
         <v>375</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3785,7 +3785,7 @@
         <v>362</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -3793,7 +3793,7 @@
         <v>363</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3801,7 +3801,7 @@
         <v>365</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3809,7 +3809,7 @@
         <v>387</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -3817,7 +3817,7 @@
         <v>386</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3825,7 +3825,7 @@
         <v>388</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3833,7 +3833,7 @@
         <v>379</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3841,7 +3841,7 @@
         <v>380</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
         <v>381</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3857,7 +3857,7 @@
         <v>382</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
         <v>360</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -3873,7 +3873,7 @@
         <v>377</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -3881,7 +3881,7 @@
         <v>368</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3889,7 +3889,7 @@
         <v>367</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3897,7 +3897,7 @@
         <v>371</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -3905,7 +3905,7 @@
         <v>372</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="375" x14ac:dyDescent="0.25">
@@ -3913,7 +3913,7 @@
         <v>370</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -3921,7 +3921,7 @@
         <v>389</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -3929,15 +3929,15 @@
         <v>390</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>453</v>
+        <v>403</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -3945,15 +3945,15 @@
         <v>397</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>450</v>
+        <v>401</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3961,7 +3961,7 @@
         <v>334</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3969,7 +3969,7 @@
         <v>335</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3977,7 +3977,7 @@
         <v>332</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>399</v>
+        <v>442</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -3985,7 +3985,7 @@
         <v>336</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -3993,7 +3993,7 @@
         <v>337</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4001,7 +4001,7 @@
         <v>338</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4009,7 +4009,7 @@
         <v>326</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4017,7 +4017,7 @@
         <v>339</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4025,7 +4025,7 @@
         <v>340</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4033,7 +4033,7 @@
         <v>343</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4041,7 +4041,7 @@
         <v>323</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4049,7 +4049,7 @@
         <v>341</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4057,7 +4057,7 @@
         <v>327</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -4065,7 +4065,7 @@
         <v>328</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4073,7 +4073,7 @@
         <v>329</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4081,7 +4081,7 @@
         <v>330</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -4089,7 +4089,7 @@
         <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>457</v>
+        <v>406</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4121,7 +4121,7 @@
         <v>346</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -4129,7 +4129,7 @@
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>455</v>
+        <v>404</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4409,7 +4409,7 @@
         <v>391</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4457,7 +4457,7 @@
         <v>8</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>447</v>
+        <v>399</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4489,7 +4489,7 @@
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>452</v>
+        <v>402</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4697,7 +4697,7 @@
         <v>89</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>456</v>
+        <v>405</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="165" x14ac:dyDescent="0.25">

</xml_diff>